<commit_message>
spreadsheet: add ability to recalculate formulas
If the formula executes without errors, it stores the
result as a cached value in the sheet.
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/formula/formula.xlsx
+++ b/_examples/spreadsheet/formula/formula.xlsx
@@ -186,9 +186,10 @@
       </ma:c>
     </ma:row>
     <ma:row r="12">
-      <ma:c r="A12"/>
-      <ma:c r="B12" t="str">
+      <ma:c r="A12" t="n"/>
+      <ma:c r="B12" t="inlineStr">
         <ma:f>SUM(B2:B11)</ma:f>
+        <ma:v>55</ma:v>
       </ma:c>
     </ma:row>
   </ma:sheetData>

</xml_diff>